<commit_message>
Q223 earnings update - maintain
</commit_message>
<xml_diff>
--- a/MSFT.xlsx
+++ b/MSFT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremyjiao/Desktop/GitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A619E5F8-740D-4440-9CA0-BE63C65C4F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AB3B40-5699-D24A-A022-27354A02133E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="19240" xr2:uid="{2E5D1925-16E4-6343-BB2A-99E1D0854617}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19240" activeTab="1" xr2:uid="{2E5D1925-16E4-6343-BB2A-99E1D0854617}"/>
   </bookViews>
   <sheets>
     <sheet name="DCF" sheetId="2" r:id="rId1"/>
@@ -41,6 +41,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={EA43DE6B-0504-B945-A511-E3D3287746A0}</author>
+    <author>tc={80BB8829-8127-6A49-AACD-91E7FFE5C339}</author>
   </authors>
   <commentList>
     <comment ref="M2" authorId="0" shapeId="0" xr:uid="{EA43DE6B-0504-B945-A511-E3D3287746A0}">
@@ -62,6 +63,15 @@
 Other income: $200m
 Effective tax rate: 19% - 20%
 </t>
+      </text>
+    </comment>
+    <comment ref="L27" authorId="1" shapeId="0" xr:uid="{80BB8829-8127-6A49-AACD-91E7FFE5C339}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Q223 comments: Price target $307 to $298, nothing really crazy happened in the earnings call, mainly I had to adjust way down on the revenue expectation of the device &amp; window segment since it's expected to decline to pre-pandemic levels. Q323 guidance was a little bit disappointing, although most of it was inline with my projections, however, gross margin is expected to decline by 1-2%, OpEx increase 11% - 12% while revenue is only expected to increase 7% - little bit of a red flag there, but I still kept my 2027 43% Operating margin's target since I don't think this quarters margin was too out of wack unlike META and GOOGL. And I think 3% OpInc margin increase is totally durable given Microsoft's strong financial discipline (thanks to Amy Hood), as well as past financial performance.
+Overall, I would still maintain a buy rating since it has an implied upside of 24% and I still believe MSFT is one of that best company out there in tech, speaking of industry attractiveness, competitive advantage, pricing power and I do believe MSFT's valuation is fairly attractive compared to it's peer.</t>
       </text>
     </comment>
   </commentList>
@@ -651,7 +661,7 @@
     <numFmt numFmtId="167" formatCode="General\A"/>
     <numFmt numFmtId="168" formatCode="General\E"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -830,6 +840,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -2190,6 +2206,10 @@
 Effective tax rate: 19% - 20%
 </text>
   </threadedComment>
+  <threadedComment ref="L27" dT="2023-01-25T05:15:30.18" personId="{069DB50F-6F6B-8848-B602-971B1A970163}" id="{80BB8829-8127-6A49-AACD-91E7FFE5C339}">
+    <text>Q223 comments: Price target $307 to $298, nothing really crazy happened in the earnings call, mainly I had to adjust way down on the revenue expectation of the device &amp; window segment since it's expected to decline to pre-pandemic levels. Q323 guidance was a little bit disappointing, although most of it was inline with my projections, however, gross margin is expected to decline by 1-2%, OpEx increase 11% - 12% while revenue is only expected to increase 7% - little bit of a red flag there, but I still kept my 2027 43% Operating margin's target since I don't think this quarters margin was too out of wack unlike META and GOOGL. And I think 3% OpInc margin increase is totally durable given Microsoft's strong financial discipline (thanks to Amy Hood), as well as past financial performance.
+Overall, I would still maintain a buy rating since it has an implied upside of 24% and I still believe MSFT is one of that best company out there in tech, speaking of industry attractiveness, competitive advantage, pricing power and I do believe MSFT's valuation is fairly attractive compared to it's peer.</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2197,7 +2217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE2E371-8AA1-F249-831E-54B4381FEF21}">
   <dimension ref="A2:AA146"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -7890,7 +7910,7 @@
       <c r="E146" s="72"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="DpXs24lMpmZBJ2GiPGDV8Ytt9mF2FHYAnFC9C8da7VQqaUM3C/761S7cyT6pOR2EpRv9wb1tC0XxH0Zm/+oQGg==" saltValue="FQU2lJvmIOuPi7H4kUYNKw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="v9m92ydzif2uuRiUZBDMaNm6kPAqmkNo8Nx33S45QA6+WV033UaCQYpSYyP+AtVYlvw94/8tCx+qCXFuiveT4Q==" saltValue="Y1KjZlyqsCKGGjC0TITQZQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="4">
     <mergeCell ref="D119:H120"/>
     <mergeCell ref="L119:P120"/>
@@ -7908,12 +7928,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA1C70B-88C4-3D40-B1FA-FBB2310A7FE3}">
   <dimension ref="B1:EZ63"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="U46" sqref="U46"/>
       <selection pane="topRight" activeCell="U46" sqref="U46"/>
       <selection pane="bottomLeft" activeCell="U46" sqref="U46"/>
-      <selection pane="bottomRight" activeCell="R31" sqref="R31"/>
+      <selection pane="bottomRight" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13751,7 +13771,7 @@
       <c r="AG63" s="34"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="QMNNprWB034JsDXNqjUN8i/X72q5X0dJbptrAkcOmxY0FOY8MeL1GvgthrRYv6GB/uzvQmgWSOiXh4/wfFmXNg==" saltValue="tc5vqgEbglK+lfwawq3few==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="5dk+rWHuGCiHQOj+7/hkxlpGI5Dg9DxuCa9GrIyc1oneUxhHF+3cYRHS6v8AGyKVwFs7XxKzlB18jTs/cddwnQ==" saltValue="UzusB9p4QQRi2b+5gE5j6g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="T17 V19 G55 S55 T55:X55 H55:O55" formulaRange="1"/>

</xml_diff>